<commit_message>
modified:   deployment_manifests/pdql_manifest.csv 	modified:   "\320\270\321\201\321\205\320\276\320\264\320\275\321\213\320\265 \320\274\320\260\320\275\320\270\321\204\320\265\321\201\321\202\321\213/pdql_manifest.xlsx"
</commit_message>
<xml_diff>
--- a/исходные манифесты/pdql_manifest.xlsx
+++ b/исходные манифесты/pdql_manifest.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20408"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AD1A17E-53F0-4A06-BC06-A62E7DD5E85A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7567770-387B-49D3-ADE5-B6685057D18A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="52">
   <si>
     <t>А_Группировка по ОС</t>
   </si>
@@ -40,9 +40,6 @@
     <t>none</t>
   </si>
   <si>
-    <t>select(@Host, Host.@Name, Host.@Importance, Host.OsName,select(@Host, Host.@Name, Host.@Importance, Host.OsName, Host.@CreationTime, Host.@UpdateTime) | group(Host.OsName, COUNT(@Host)) Host.@CreationTime, Host.@UpdateTime) | group(Host.OsName, COUNT(@Host))</t>
-  </si>
-  <si>
     <t>common</t>
   </si>
   <si>
@@ -121,9 +118,6 @@
     <t>А_Успешный пентест</t>
   </si>
   <si>
-    <t>select(@Host, Host.@Importance as Imprt, Host.@Vulners as Vulner, Host.@Vulners.DiscoveryTime as Discovered, Host.@Vulners.Description as Description, Host.@Vulners.HowToFix as Fix, Host.@Vulners.Status, Host.@Vulners.StatusUpdateTime as UpdateTime, Host.@Vulners.DueTime as SolveBefore) | filter(Vulner like "Подобраны%")</t>
-  </si>
-  <si>
     <t>А_ Сканирование было давно</t>
   </si>
   <si>
@@ -151,9 +145,6 @@
     <t>А_ Было ли сканирование</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>false</t>
   </si>
   <si>
@@ -191,6 +182,12 @@
   </si>
   <si>
     <t>тип</t>
+  </si>
+  <si>
+    <t>select(@Host, Host.@Name, Host.@Importance, Host.OsName, Host.@CreationTime, Host.@UpdateTime) | group(Host.OsName, COUNT(@Host))</t>
+  </si>
+  <si>
+    <t>select(@Host, Host.OsName, Host.@CreationTime, Host.@UpdateTime, Host.Endpoints&lt;TransportEndpoint&gt;.Service.Checks&lt;RemoteAccessAccountBruteforce&gt;.Login as login, Host.Endpoints&lt;TransportEndpoint&gt;.Service.Checks&lt;RemoteAccessAccountBruteforce&gt;.Password as password) | filter(Login or password)</t>
   </si>
 </sst>
 </file>
@@ -226,9 +223,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -292,9 +292,9 @@
     <tableColumn id="2" xr3:uid="{5C2FEDED-F5B7-4C75-B2B3-3BB0F6E876D7}" uniqueName="2" name="Префильтрация" queryTableFieldId="2" dataDxfId="5"/>
     <tableColumn id="3" xr3:uid="{781C2E06-194E-4BCB-BCA3-10BB69AC3D68}" uniqueName="3" name="Группа в которой находится запрос" queryTableFieldId="3" dataDxfId="4"/>
     <tableColumn id="4" xr3:uid="{8BF9801E-1945-4FF3-83DE-23D0D0588612}" uniqueName="4" name="Удален" queryTableFieldId="4" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{472F2C3A-DF2D-4B91-8293-9E57FA928AEA}" uniqueName="5" name="Инвалидный" queryTableFieldId="5" dataDxfId="0"/>
-    <tableColumn id="6" xr3:uid="{6B9A9C56-87B3-4DC9-B344-B605F6968EC9}" uniqueName="6" name="PDQL запрос" queryTableFieldId="6" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{8182C634-62B6-4B6C-A04F-27E0B9F547A7}" uniqueName="7" name="тип" queryTableFieldId="7" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{472F2C3A-DF2D-4B91-8293-9E57FA928AEA}" uniqueName="5" name="Инвалидный" queryTableFieldId="5" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{6B9A9C56-87B3-4DC9-B344-B605F6968EC9}" uniqueName="6" name="PDQL запрос" queryTableFieldId="6" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{8182C634-62B6-4B6C-A04F-27E0B9F547A7}" uniqueName="7" name="тип" queryTableFieldId="7" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -567,7 +567,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -577,45 +577,45 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F89869B2-D76D-4540-AD9F-245A567F0AC5}">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.1796875" customWidth="1"/>
-    <col min="3" max="3" width="34.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="81.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="81.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -623,252 +623,252 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="D4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="D5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="1" t="s">
+      <c r="G5" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
+      <c r="B6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
+      <c r="B7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
+      <c r="B8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
+      <c r="B9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F9" s="1" t="s">
+      <c r="G9" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
+      <c r="B10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F10" s="1" t="s">
+      <c r="G10" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
+      <c r="B11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F11" s="1" t="s">
+      <c r="G11" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
+      <c r="B12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="G12" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>0</v>
       </c>
@@ -876,180 +876,180 @@
         <v>1</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
+      <c r="D15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F15" s="1" t="s">
+      <c r="B16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G15" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F16" s="1" t="s">
+      <c r="G17" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G16" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F17" s="1" t="s">
+      <c r="G18" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G17" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F18" s="1" t="s">
+      <c r="G19" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F20" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G18" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A19" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="G20" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>